<commit_message>
Added code to HandleUntrustedConnection for Admin, Fixed code to user Appsettings key types instead of handling it as string, removed Delays in all pages except Public_NewAcctAccess.cs, cleaned commented code, Enhanced  ExcelData.read method and removed Testdata folder - for properly running from commandline
</commit_message>
<xml_diff>
--- a/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/Admin_CS_NewAcctData.xlsx
+++ b/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/Admin_CS_NewAcctData.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -57,9 +57,6 @@
     <t>RenewSame</t>
   </si>
   <si>
-    <t>Ben Miller</t>
-  </si>
-  <si>
     <t>lyndaCampus admin</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>lyndaEnterprise admin</t>
+  </si>
+  <si>
+    <t>Carin Richard</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="B1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
         <v>12</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1">
         <v>41014</v>
@@ -497,7 +497,7 @@
         <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
         <v>12</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1">
         <v>41014</v>
@@ -517,7 +517,7 @@
         <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1">
         <v>41014</v>
@@ -537,7 +537,7 @@
         <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>

</xml_diff>